<commit_message>
ft: added pattern generator && param generator with unit test
</commit_message>
<xml_diff>
--- a/data/campeonato_prueba.xlsx
+++ b/data/campeonato_prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdduarte/Development/universidad/tesis/calendar-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9429280F-079B-1A4A-813E-C200276582C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A110E0-FBDF-184D-9B95-1FE5BEBAFC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="3">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -440,7 +440,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -474,7 +474,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -491,7 +491,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -508,7 +508,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>

</xml_diff>